<commit_message>
file excel download in progress
</commit_message>
<xml_diff>
--- a/listedepoints.xlsx
+++ b/listedepoints.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="19">
   <si>
     <t>Sous-ensemble</t>
   </si>
@@ -52,12 +52,6 @@
     <t xml:space="preserve">Commande chaudiere </t>
   </si>
   <si>
-    <t>Chaudière 2</t>
-  </si>
-  <si>
-    <t>Chaudière 3</t>
-  </si>
-  <si>
     <t>Circuit Régulé 1</t>
   </si>
   <si>
@@ -67,9 +61,6 @@
     <t>Commande V3V 1</t>
   </si>
   <si>
-    <t>Circuit Régulé 2</t>
-  </si>
-  <si>
     <t>Général</t>
   </si>
   <si>
@@ -79,7 +70,7 @@
     <t xml:space="preserve">Défaut manque d'eau </t>
   </si>
   <si>
-    <t xml:space="preserve"> TOTAUX (32 points)</t>
+    <t xml:space="preserve"> TOTAUX (14 points)</t>
   </si>
 </sst>
 </file>
@@ -440,7 +431,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G29"/>
+  <dimension ref="A1:G14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -602,13 +593,13 @@
         <v>12</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="C8" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D8" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E8" s="2">
         <v>0</v>
@@ -665,7 +656,7 @@
         <v>12</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="C11" s="2">
         <v>0</v>
@@ -674,19 +665,19 @@
         <v>0</v>
       </c>
       <c r="E11" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F11" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G11" s="2"/>
     </row>
     <row r="12" spans="1:7">
       <c r="A12" s="2" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="C12" s="2">
         <v>1</v>
@@ -704,10 +695,10 @@
     </row>
     <row r="13" spans="1:7">
       <c r="A13" s="2" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="C13" s="2">
         <v>0</v>
@@ -724,338 +715,23 @@
       <c r="G13" s="2"/>
     </row>
     <row r="14" spans="1:7">
-      <c r="A14" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C14" s="2">
-        <v>0</v>
-      </c>
-      <c r="D14" s="2">
-        <v>1</v>
-      </c>
-      <c r="E14" s="2">
-        <v>0</v>
-      </c>
-      <c r="F14" s="2">
-        <v>0</v>
-      </c>
-      <c r="G14" s="2"/>
-    </row>
-    <row r="15" spans="1:7">
-      <c r="A15" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C15" s="2">
-        <v>0</v>
-      </c>
-      <c r="D15" s="2">
-        <v>0</v>
-      </c>
-      <c r="E15" s="2">
-        <v>1</v>
-      </c>
-      <c r="F15" s="2">
-        <v>1</v>
-      </c>
-      <c r="G15" s="2"/>
-    </row>
-    <row r="16" spans="1:7">
-      <c r="A16" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C16" s="2">
-        <v>0</v>
-      </c>
-      <c r="D16" s="2">
-        <v>0</v>
-      </c>
-      <c r="E16" s="2">
-        <v>0</v>
-      </c>
-      <c r="F16" s="2">
-        <v>1</v>
-      </c>
-      <c r="G16" s="2"/>
-    </row>
-    <row r="17" spans="1:7">
-      <c r="A17" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C17" s="2">
-        <v>1</v>
-      </c>
-      <c r="D17" s="2">
-        <v>0</v>
-      </c>
-      <c r="E17" s="2">
-        <v>0</v>
-      </c>
-      <c r="F17" s="2">
-        <v>0</v>
-      </c>
-      <c r="G17" s="2"/>
-    </row>
-    <row r="18" spans="1:7">
-      <c r="A18" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B18" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C18" s="2">
-        <v>1</v>
-      </c>
-      <c r="D18" s="2">
-        <v>0</v>
-      </c>
-      <c r="E18" s="2">
-        <v>0</v>
-      </c>
-      <c r="F18" s="2">
-        <v>0</v>
-      </c>
-      <c r="G18" s="2"/>
-    </row>
-    <row r="19" spans="1:7">
-      <c r="A19" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B19" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C19" s="2">
-        <v>0</v>
-      </c>
-      <c r="D19" s="2">
-        <v>1</v>
-      </c>
-      <c r="E19" s="2">
-        <v>0</v>
-      </c>
-      <c r="F19" s="2">
-        <v>0</v>
-      </c>
-      <c r="G19" s="2"/>
-    </row>
-    <row r="20" spans="1:7">
-      <c r="A20" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B20" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C20" s="2">
-        <v>0</v>
-      </c>
-      <c r="D20" s="2">
-        <v>0</v>
-      </c>
-      <c r="E20" s="2">
-        <v>1</v>
-      </c>
-      <c r="F20" s="2">
-        <v>1</v>
-      </c>
-      <c r="G20" s="2"/>
-    </row>
-    <row r="21" spans="1:7">
-      <c r="A21" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B21" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="C21" s="2">
-        <v>0</v>
-      </c>
-      <c r="D21" s="2">
-        <v>0</v>
-      </c>
-      <c r="E21" s="2">
-        <v>1</v>
-      </c>
-      <c r="F21" s="2">
-        <v>0</v>
-      </c>
-      <c r="G21" s="2"/>
-    </row>
-    <row r="22" spans="1:7">
-      <c r="A22" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B22" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C22" s="2">
-        <v>1</v>
-      </c>
-      <c r="D22" s="2">
-        <v>0</v>
-      </c>
-      <c r="E22" s="2">
-        <v>0</v>
-      </c>
-      <c r="F22" s="2">
-        <v>0</v>
-      </c>
-      <c r="G22" s="2"/>
-    </row>
-    <row r="23" spans="1:7">
-      <c r="A23" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B23" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C23" s="2">
-        <v>1</v>
-      </c>
-      <c r="D23" s="2">
-        <v>0</v>
-      </c>
-      <c r="E23" s="2">
-        <v>0</v>
-      </c>
-      <c r="F23" s="2">
-        <v>0</v>
-      </c>
-      <c r="G23" s="2"/>
-    </row>
-    <row r="24" spans="1:7">
-      <c r="A24" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B24" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C24" s="2">
-        <v>0</v>
-      </c>
-      <c r="D24" s="2">
-        <v>1</v>
-      </c>
-      <c r="E24" s="2">
-        <v>0</v>
-      </c>
-      <c r="F24" s="2">
-        <v>0</v>
-      </c>
-      <c r="G24" s="2"/>
-    </row>
-    <row r="25" spans="1:7">
-      <c r="A25" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B25" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C25" s="2">
-        <v>0</v>
-      </c>
-      <c r="D25" s="2">
-        <v>0</v>
-      </c>
-      <c r="E25" s="2">
-        <v>1</v>
-      </c>
-      <c r="F25" s="2">
-        <v>1</v>
-      </c>
-      <c r="G25" s="2"/>
-    </row>
-    <row r="26" spans="1:7">
-      <c r="A26" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B26" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="C26" s="2">
-        <v>0</v>
-      </c>
-      <c r="D26" s="2">
-        <v>0</v>
-      </c>
-      <c r="E26" s="2">
-        <v>1</v>
-      </c>
-      <c r="F26" s="2">
-        <v>0</v>
-      </c>
-      <c r="G26" s="2"/>
-    </row>
-    <row r="27" spans="1:7">
-      <c r="A27" s="2" t="s">
+      <c r="A14" s="1"/>
+      <c r="B14" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B27" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="C27" s="2">
-        <v>1</v>
-      </c>
-      <c r="D27" s="2">
-        <v>0</v>
-      </c>
-      <c r="E27" s="2">
-        <v>0</v>
-      </c>
-      <c r="F27" s="2">
-        <v>0</v>
-      </c>
-      <c r="G27" s="2"/>
-    </row>
-    <row r="28" spans="1:7">
-      <c r="A28" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="B28" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="C28" s="2">
-        <v>0</v>
-      </c>
-      <c r="D28" s="2">
-        <v>1</v>
-      </c>
-      <c r="E28" s="2">
-        <v>0</v>
-      </c>
-      <c r="F28" s="2">
-        <v>0</v>
-      </c>
-      <c r="G28" s="2"/>
-    </row>
-    <row r="29" spans="1:7">
-      <c r="A29" s="1"/>
-      <c r="B29" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C29" s="1">
-        <v>8</v>
-      </c>
-      <c r="D29" s="1">
-        <v>9</v>
-      </c>
-      <c r="E29" s="1">
-        <v>7</v>
-      </c>
-      <c r="F29" s="1">
-        <v>8</v>
-      </c>
-      <c r="G29" s="1"/>
+      <c r="C14" s="1">
+        <v>4</v>
+      </c>
+      <c r="D14" s="1">
+        <v>4</v>
+      </c>
+      <c r="E14" s="1">
+        <v>3</v>
+      </c>
+      <c r="F14" s="1">
+        <v>3</v>
+      </c>
+      <c r="G14" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>